<commit_message>
GUI: Updated the statistics.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/_Test_Suite_Statistics_for_Folders.xlsx
+++ b/QA/Tests/CRUD/Create/_Test_Suite_Statistics_for_Folders.xlsx
@@ -326,22 +326,22 @@
             <v>13</v>
           </cell>
           <cell r="G1">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="2">
           <cell r="G2">
-            <v>10</v>
+            <v>11</v>
           </cell>
         </row>
         <row r="4">
           <cell r="G4">
-            <v>91</v>
+            <v>98</v>
           </cell>
         </row>
         <row r="5">
           <cell r="G5">
-            <v>58</v>
+            <v>75</v>
           </cell>
         </row>
       </sheetData>
@@ -716,7 +716,7 @@
       </c>
       <c r="H2" s="4">
         <f>SUM($B:$B)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>1</v>
@@ -755,7 +755,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM($C:$C)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I3" s="3"/>
     </row>
@@ -793,11 +793,11 @@
       </c>
       <c r="B5" s="1">
         <f>[4]Sheet1!$G$1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
         <f>[4]Sheet1!$G$2</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1">
         <f>[4]Sheet1!$E$1</f>
@@ -805,18 +805,18 @@
       </c>
       <c r="E5" s="1">
         <f>[4]Sheet1!$G$5</f>
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="F5" s="1">
         <f>[4]Sheet1!$G$4</f>
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="4">
         <f xml:space="preserve"> SUM($F:$F)</f>
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="I5" s="3"/>
     </row>
@@ -826,7 +826,7 @@
       </c>
       <c r="H6" s="4">
         <f xml:space="preserve"> SUM($E:$E)</f>
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="I6" s="3"/>
     </row>
@@ -836,7 +836,7 @@
       </c>
       <c r="H7" s="7">
         <f>H6/H5</f>
-        <v>0.76470588235294112</v>
+        <v>0.81578947368421051</v>
       </c>
       <c r="I7" s="3"/>
     </row>

</xml_diff>